<commit_message>
spliting data to schemas
</commit_message>
<xml_diff>
--- a/public/Коды маркировки.xlsx
+++ b/public/Коды маркировки.xlsx
@@ -465,7 +465,7 @@
   <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -491,7 +491,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1">
         <v>5501234567891</v>
@@ -504,7 +504,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="1">
         <v>5501234567891</v>
@@ -517,7 +517,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="1">
         <v>5501234567891</v>
@@ -530,7 +530,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" s="1">
         <v>5501234567891</v>
@@ -543,7 +543,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B6" s="1">
         <v>5501234567891</v>
@@ -556,7 +556,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B7" s="1">
         <v>5501234567891</v>
@@ -569,7 +569,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B8" s="1">
         <v>5501234567891</v>
@@ -582,7 +582,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B9" s="1">
         <v>5501234567891</v>
@@ -595,7 +595,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B10" s="1">
         <v>5501234567891</v>
@@ -608,7 +608,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B11" s="1">
         <v>5501234567891</v>
@@ -621,7 +621,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B12" s="1">
         <v>5501234567891</v>
@@ -634,7 +634,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B13" s="1">
         <v>5501234567891</v>
@@ -647,7 +647,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B14" s="1">
         <v>5501234567891</v>
@@ -660,7 +660,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B15" s="1">
         <v>5501234567891</v>
@@ -673,7 +673,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B16" s="1">
         <v>5501234567891</v>
@@ -686,7 +686,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B17" s="1">
         <v>5501234567891</v>
@@ -699,7 +699,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B18" s="1">
         <v>5501234567891</v>
@@ -712,7 +712,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B19" s="1">
         <v>5501234567891</v>
@@ -725,7 +725,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B20" s="1">
         <v>5501234567891</v>
@@ -738,7 +738,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B21" s="1">
         <v>5501234567892</v>
@@ -751,7 +751,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B22" s="1">
         <v>5501234567892</v>
@@ -764,7 +764,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B23" s="1">
         <v>5501234567892</v>
@@ -777,7 +777,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B24" s="1">
         <v>5501234567892</v>
@@ -790,7 +790,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B25" s="1">
         <v>5501234567892</v>
@@ -803,7 +803,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B26" s="1">
         <v>5501234567892</v>
@@ -816,7 +816,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B27" s="1">
         <v>5501234567892</v>
@@ -829,7 +829,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B28" s="1">
         <v>5501234567892</v>
@@ -842,7 +842,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B29" s="1">
         <v>5501234567892</v>
@@ -855,7 +855,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B30" s="1">
         <v>5501234567892</v>
@@ -868,7 +868,7 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B31" s="1">
         <v>5501234567892</v>

</xml_diff>